<commit_message>
V2.0 add substation_info and configuration
</commit_message>
<xml_diff>
--- a/bidding_web.xlsx
+++ b/bidding_web.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22325"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B66537B3-AE77-42B6-B3FD-7BB8A116F0C3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB603F99-0F32-434C-875B-430500E8FC11}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>http://www.cgdcbidding.com/ggsb/index.jhtml</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -131,6 +131,26 @@
   </si>
   <si>
     <t>文件名</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>中国南方电网</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://www.bidding.csg.cn/zbgg/index.jhtml</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://ebidding.sinopec.com/TPWeb4AAA/jyxx/002002/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>中国石化</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>中国石油</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -221,9 +241,6 @@
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -232,6 +249,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -573,10 +593,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -587,137 +607,162 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="39.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="5" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A3" s="1"/>
-      <c r="B3" s="2" t="s">
+      <c r="A3" s="5"/>
+      <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="1"/>
+      <c r="C3" s="5"/>
     </row>
     <row r="4" spans="1:3" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A4" s="1"/>
-      <c r="B4" s="2" t="s">
+      <c r="A4" s="5"/>
+      <c r="B4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="1"/>
+      <c r="C4" s="5"/>
     </row>
     <row r="5" spans="1:3" ht="66" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="2" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="5" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A7" s="1"/>
-      <c r="B7" s="4" t="s">
+      <c r="A7" s="5"/>
+      <c r="B7" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="1"/>
+      <c r="C7" s="5"/>
     </row>
     <row r="8" spans="1:3" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" s="5" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A9" s="1"/>
-      <c r="B9" s="4" t="s">
+      <c r="A9" s="5"/>
+      <c r="B9" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="1"/>
+      <c r="C9" s="5"/>
     </row>
     <row r="10" spans="1:3" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="2" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
+      <c r="A11" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" s="5" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A12" s="1"/>
-      <c r="B12" s="2" t="s">
+      <c r="A12" s="5"/>
+      <c r="B12" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C12" s="1"/>
+      <c r="C12" s="5"/>
     </row>
     <row r="13" spans="1:3" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A13" s="1"/>
-      <c r="B13" s="2" t="s">
+      <c r="A13" s="5"/>
+      <c r="B13" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C13" s="1"/>
+      <c r="C13" s="5"/>
     </row>
     <row r="14" spans="1:3" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A14" s="1"/>
-      <c r="B14" s="2" t="s">
+      <c r="A14" s="5"/>
+      <c r="B14" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C14" s="1"/>
+      <c r="C14" s="5"/>
     </row>
     <row r="15" spans="1:3" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A15" s="1"/>
-      <c r="B15" s="2" t="s">
+      <c r="A15" s="5"/>
+      <c r="B15" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C15" s="1"/>
+      <c r="C15" s="5"/>
+    </row>
+    <row r="16" spans="1:3" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C16" s="2"/>
+    </row>
+    <row r="17" spans="1:3" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C17" s="2"/>
+    </row>
+    <row r="18" spans="1:3" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B18" s="1"/>
+      <c r="C18" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -746,9 +791,11 @@
     <hyperlink ref="B13" r:id="rId12" xr:uid="{E8B5370C-9416-4062-953A-2D603704441A}"/>
     <hyperlink ref="B14" r:id="rId13" xr:uid="{686B6077-29A4-4493-8A6A-6BEA86659A46}"/>
     <hyperlink ref="B15" r:id="rId14" xr:uid="{B2924C08-E3C4-4748-8BAF-2819A132AC20}"/>
+    <hyperlink ref="B16" r:id="rId15" xr:uid="{22D6980E-10FE-434E-8606-D8DF564AAB83}"/>
+    <hyperlink ref="B17" r:id="rId16" xr:uid="{0BF1ECBE-BE65-4350-AA7D-5E7E193D3F63}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId15"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId17"/>
 </worksheet>
 </file>
 

</xml_diff>